<commit_message>
EPBDS-7990 return type validation must be skipped if method has ServiceCallAroundInterceptor annotation
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebServiceAnnotation/openl-repository/deployments/ws-serviceclass-positive/ws-serviceclass-positive/main.xlsx
+++ b/ITEST/itest.WebServiceAnnotation/openl-repository/deployments/ws-serviceclass-positive/ws-serviceclass-positive/main.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>return Long.valueOf(str);</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Method Long longMethodWithUpcast(String str)</t>
+  </si>
+  <si>
+    <t>Method Long aroundLongMethod(String str)</t>
+  </si>
+  <si>
+    <t>Method void aroundVoidMethod()</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B24"/>
+  <dimension ref="B4:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,6 +437,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>